<commit_message>
Subo devuelta la estimacion de documentacion
</commit_message>
<xml_diff>
--- a/doc/Interno/Estimación Tiempos Documentación (En construcción).xlsx
+++ b/doc/Interno/Estimación Tiempos Documentación (En construcción).xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juli\Google Drive\Proyecto Final\Interno\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>ESTIMACION TIEMPOS DOCUMENTACION</t>
   </si>
@@ -59,9 +54,6 @@
     <t>Diagrama de Arquitectura</t>
   </si>
   <si>
-    <t>Documento de Factibilidad Economica</t>
-  </si>
-  <si>
     <t>Documento de Lecciones Aprendidas</t>
   </si>
   <si>
@@ -77,24 +69,9 @@
     <t>Especificacion de Casos de Uso</t>
   </si>
   <si>
-    <t>Especificacion Funcional</t>
-  </si>
-  <si>
-    <t>Trazabilidad</t>
-  </si>
-  <si>
-    <t>Casos de Prueba</t>
-  </si>
-  <si>
-    <t>Plan de Prueba</t>
-  </si>
-  <si>
     <t>Diagramas de clase</t>
   </si>
   <si>
-    <t>Minutas de Reunion</t>
-  </si>
-  <si>
     <t>TIEMPO (Hs)</t>
   </si>
   <si>
@@ -107,12 +84,6 @@
     <t>ANALISIS</t>
   </si>
   <si>
-    <t>CODIFICACION</t>
-  </si>
-  <si>
-    <t>PRUEBA</t>
-  </si>
-  <si>
     <t>IMPLEMENTACION</t>
   </si>
   <si>
@@ -122,47 +93,83 @@
     <t>Informe de Estudio de Mercado</t>
   </si>
   <si>
-    <t>Revisiones periodicas y correccion de desvios</t>
-  </si>
-  <si>
     <t>COMENTARIOS</t>
   </si>
   <si>
-    <t>Por cada etapa se completa el Acta</t>
-  </si>
-  <si>
     <t>Acta de Constitucion de Proyecto</t>
   </si>
   <si>
-    <t>Presupuesto</t>
-  </si>
-  <si>
     <t>Diccionario de Datos</t>
   </si>
   <si>
-    <t>NOSE QUE ES ESTO jaja</t>
-  </si>
-  <si>
-    <t>LOS ENTREGABLES SERIAN LOS DETALLADOS POR</t>
-  </si>
-  <si>
-    <t>ALEX Y PABLO EN EL DOCUMENTO DE DESARROLLO</t>
-  </si>
-  <si>
     <t>DISEÑO</t>
   </si>
   <si>
-    <t>Acá estaría bueno poner algo relacionado</t>
-  </si>
-  <si>
-    <t>al márketing… diseño de poster, logo, merchandising….</t>
+    <t>si</t>
+  </si>
+  <si>
+    <t>Estimación de Costos</t>
+  </si>
+  <si>
+    <t>Documento de Factibilidad Economica, Tecnica y Operativa</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Manual de usuario para supermercado</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Modulos ABM Productos</t>
+  </si>
+  <si>
+    <t>Modulos Login</t>
+  </si>
+  <si>
+    <t>Modulos Mapas</t>
+  </si>
+  <si>
+    <t>Modulos ABM Promociones</t>
+  </si>
+  <si>
+    <t>Modulos Listas de compras</t>
+  </si>
+  <si>
+    <t>Modulos Compras</t>
+  </si>
+  <si>
+    <t>Modulos Navegación</t>
+  </si>
+  <si>
+    <t>Modulo Notificaciones</t>
+  </si>
+  <si>
+    <t>Modulo Estadistica</t>
+  </si>
+  <si>
+    <t>Modulo Gestión de Mapas</t>
+  </si>
+  <si>
+    <t>Modulo Operador por voz</t>
+  </si>
+  <si>
+    <t>Modulo Gestion TAG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +189,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -214,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -223,6 +234,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Celda vinculada" xfId="1" builtinId="24"/>
@@ -284,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,7 +331,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,233 +508,323 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" customHeight="1" thickTop="1">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" customHeight="1"/>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.5">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="25.5">
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="C32" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="C33" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="C39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>